<commit_message>
SRS-2022: Changed order of response alternatives for SA_1_gross to be in sequential order
</commit_message>
<xml_diff>
--- a/web/src/main/resources/SRS_PM_indata_3_0.xlsx
+++ b/web/src/main/resources/SRS_PM_indata_3_0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian/Development/inera/intyg/srs/web/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881575D3-7891-4C4B-83F2-B3716F62ADC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659029FE-7955-744C-B643-EC2BDEF21374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9160" yWindow="10180" windowWidth="24440" windowHeight="30420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8060" yWindow="7480" windowWidth="22980" windowHeight="30320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kodning av variabelnamn" sheetId="1" r:id="rId1"/>
@@ -1316,8 +1316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1668,7 +1668,7 @@
         <v>73</v>
       </c>
       <c r="D23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E23" t="s">
         <v>55</v>
@@ -1685,7 +1685,7 @@
         <v>75</v>
       </c>
       <c r="D24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E24" t="s">
         <v>55</v>
@@ -1910,7 +1910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <selection activeCell="E163" sqref="E163"/>
     </sheetView>
   </sheetViews>

</xml_diff>